<commit_message>
translated chapter 6 names
</commit_message>
<xml_diff>
--- a/rownames adjusted.xlsx
+++ b/rownames adjusted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soffi\Desktop\CONSULTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807408B4-0FA4-4C41-AB4F-5B8F9C25AD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800C1A76-BC60-4FDB-9162-4A662665558E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{E99DE6AB-F055-4BDC-AA42-ACA0102CF20D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{E99DE6AB-F055-4BDC-AA42-ACA0102CF20D}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Institutes" sheetId="4" r:id="rId3"/>
     <sheet name="Institutes2" sheetId="5" r:id="rId4"/>
     <sheet name="Hierarchical" sheetId="1" r:id="rId5"/>
+    <sheet name="English" sheetId="6" r:id="rId6"/>
+    <sheet name="English2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="283">
   <si>
     <t>Algeria</t>
   </si>
@@ -850,6 +852,45 @@
   </si>
   <si>
     <t>Congregatio Total</t>
+  </si>
+  <si>
+    <t>Religious institutes (total)</t>
+  </si>
+  <si>
+    <t>ISPRs (total)</t>
+  </si>
+  <si>
+    <t>Clerical religious congregations</t>
+  </si>
+  <si>
+    <t>Lay religious congregations</t>
+  </si>
+  <si>
+    <t>Congregation for the Eastern Churches</t>
+  </si>
+  <si>
+    <t>Congregation for the Evangelization of Peoples</t>
+  </si>
+  <si>
+    <t>Congr. for the Inst. of Cons. Life and Soc. of Apos. Life</t>
+  </si>
+  <si>
+    <t>Congregations (total)</t>
+  </si>
+  <si>
+    <t>Orders - canons regular</t>
+  </si>
+  <si>
+    <t>Orders - mendicant</t>
+  </si>
+  <si>
+    <t>Orders - monastic</t>
+  </si>
+  <si>
+    <t>Orders - clerics regular</t>
+  </si>
+  <si>
+    <t>Societies of apostolic life (total)</t>
   </si>
 </sst>
 </file>
@@ -891,10 +932,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1246,7 +1286,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1254,7 +1294,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1262,7 +1302,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1270,7 +1310,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1278,7 +1318,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1286,1182 +1326,1182 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+      <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+      <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+      <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="A59" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
+      <c r="A60" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="A61" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="A62" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
+      <c r="A63" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
+      <c r="A64" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
+      <c r="A65" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
+      <c r="A66" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
+      <c r="A67" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
+      <c r="A68" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
+      <c r="A69" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
+      <c r="A70" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
+      <c r="A71" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
+      <c r="A72" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
+      <c r="A73" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
+      <c r="A74" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+      <c r="A75" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
+      <c r="A76" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
+      <c r="A77" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
+      <c r="A78" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
+      <c r="A79" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
+      <c r="A80" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
+      <c r="A81" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
+      <c r="A82" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
+      <c r="A83" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
+      <c r="A84" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
+      <c r="A85" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
+      <c r="A86" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
+      <c r="A87" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
+      <c r="A88" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
+      <c r="A89" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
+      <c r="A90" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
+      <c r="A91" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
+      <c r="A92" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
+      <c r="A93" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
+      <c r="A94" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
+      <c r="A95" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
+      <c r="A96" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="2" t="s">
+      <c r="A97" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="2" t="s">
+      <c r="A98" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="2" t="s">
+      <c r="A99" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="2" t="s">
+      <c r="A100" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
+      <c r="A101" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
+      <c r="A102" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
+      <c r="A103" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="2" t="s">
+      <c r="A104" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
+      <c r="A105" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
+      <c r="A106" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
+      <c r="A107" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
+      <c r="A108" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" s="2" t="s">
+      <c r="A109" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
+      <c r="A110" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
+      <c r="A111" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
+      <c r="A112" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
+      <c r="A113" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="2" t="s">
+      <c r="A114" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="2" t="s">
+      <c r="A115" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
+      <c r="A116" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
+      <c r="A117" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
+      <c r="A118" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
+      <c r="A119" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
+      <c r="A120" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
+      <c r="A121" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" s="2" t="s">
+      <c r="A122" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" s="2" t="s">
+      <c r="A123" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" s="2" t="s">
+      <c r="A124" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" s="2" t="s">
+      <c r="A125" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" s="2" t="s">
+      <c r="A126" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" s="2" t="s">
+      <c r="A127" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" s="2" t="s">
+      <c r="A128" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" s="2" t="s">
+      <c r="A129" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
+      <c r="A130" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="2" t="s">
+      <c r="A131" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
+      <c r="A132" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" s="2" t="s">
+      <c r="A133" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" s="2" t="s">
+      <c r="A134" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
+      <c r="A135" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" s="2" t="s">
+      <c r="A136" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
+      <c r="A137" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138" s="2" t="s">
+      <c r="A138" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" s="2" t="s">
+      <c r="A139" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" s="2" t="s">
+      <c r="A140" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141" s="2" t="s">
+      <c r="A141" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142" s="2" t="s">
+      <c r="A142" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143" s="2" t="s">
+      <c r="A143" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144" s="2" t="s">
+      <c r="A144" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145" s="2" t="s">
+      <c r="A145" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146" s="2" t="s">
+      <c r="A146" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147" s="2" t="s">
+      <c r="A147" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" s="2" t="s">
+      <c r="A148" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149" s="2" t="s">
+      <c r="A149" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150" s="2" t="s">
+      <c r="A150" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" s="2" t="s">
+      <c r="A151" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152" s="2" t="s">
+      <c r="A152" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153" s="2" t="s">
+      <c r="A153" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154" s="2" t="s">
+      <c r="A154" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155" s="2" t="s">
+      <c r="A155" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156" s="2" t="s">
+      <c r="A156" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157" s="2" t="s">
+      <c r="A157" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158" s="2" t="s">
+      <c r="A158" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A159" s="2" t="s">
+      <c r="A159" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160" s="2" t="s">
+      <c r="A160" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A161" s="2" t="s">
+      <c r="A161" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A162" s="2" t="s">
+      <c r="A162" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A163" s="2" t="s">
+      <c r="A163" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A164" s="2" t="s">
+      <c r="A164" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A165" s="2" t="s">
+      <c r="A165" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A166" s="2" t="s">
+      <c r="A166" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A167" s="2" t="s">
+      <c r="A167" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A168" s="2" t="s">
+      <c r="A168" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A169" s="2" t="s">
+      <c r="A169" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A170" s="2" t="s">
+      <c r="A170" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A171" s="2" t="s">
+      <c r="A171" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A172" s="2" t="s">
+      <c r="A172" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A173" s="2" t="s">
+      <c r="A173" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A174" s="2" t="s">
+      <c r="A174" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A175" s="2" t="s">
+      <c r="A175" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A176" s="2" t="s">
+      <c r="A176" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177" s="2" t="s">
+      <c r="A177" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A178" s="2" t="s">
+      <c r="A178" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A179" s="2" t="s">
+      <c r="A179" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A180" s="2" t="s">
+      <c r="A180" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A181" s="2" t="s">
+      <c r="A181" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A182" s="2" t="s">
+      <c r="A182" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A183" s="2" t="s">
+      <c r="A183" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A184" s="2" t="s">
+      <c r="A184" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A185" s="2" t="s">
+      <c r="A185" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A186" s="2" t="s">
+      <c r="A186" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A187" s="2" t="s">
+      <c r="A187" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A188" s="2" t="s">
+      <c r="A188" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A189" s="2" t="s">
+      <c r="A189" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A190" s="2" t="s">
+      <c r="A190" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A191" s="2" t="s">
+      <c r="A191" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A192" s="2" t="s">
+      <c r="A192" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A193" s="2" t="s">
+      <c r="A193" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A194" s="2" t="s">
+      <c r="A194" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A195" s="2" t="s">
+      <c r="A195" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A196" s="2" t="s">
+      <c r="A196" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A197" s="2" t="s">
+      <c r="A197" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A198" s="2" t="s">
+      <c r="A198" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A199" s="2" t="s">
+      <c r="A199" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A200" s="2" t="s">
+      <c r="A200" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A201" s="2" t="s">
+      <c r="A201" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A202" s="2" t="s">
+      <c r="A202" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A203" s="2" t="s">
+      <c r="A203" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A204" s="2" t="s">
+      <c r="A204" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A205" s="2" t="s">
+      <c r="A205" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A206" s="2" t="s">
+      <c r="A206" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A207" s="2" t="s">
+      <c r="A207" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A208" s="2" t="s">
+      <c r="A208" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A209" s="2" t="s">
+      <c r="A209" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A210" s="2" t="s">
+      <c r="A210" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A211" s="2" t="s">
+      <c r="A211" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A212" s="2" t="s">
+      <c r="A212" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A213" s="2" t="s">
+      <c r="A213" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A214" s="2" t="s">
+      <c r="A214" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A215" s="2" t="s">
+      <c r="A215" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A216" s="2" t="s">
+      <c r="A216" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A217" s="2" t="s">
+      <c r="A217" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A218" s="2" t="s">
+      <c r="A218" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A219" s="2" t="s">
+      <c r="A219" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A220" s="2" t="s">
+      <c r="A220" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A221" s="2" t="s">
+      <c r="A221" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A222" s="2" t="s">
+      <c r="A222" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A223" s="2" t="s">
+      <c r="A223" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A224" s="2" t="s">
+      <c r="A224" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A225" s="2" t="s">
+      <c r="A225" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A226" s="2" t="s">
+      <c r="A226" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A227" s="2" t="s">
+      <c r="A227" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A228" s="2" t="s">
+      <c r="A228" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A229" s="2" t="s">
+      <c r="A229" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A230" s="2" t="s">
+      <c r="A230" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A231" s="2" t="s">
+      <c r="A231" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A232" s="2" t="s">
+      <c r="A232" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A233" s="2" t="s">
+      <c r="A233" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A234" s="2" t="s">
+      <c r="A234" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A235" s="2" t="s">
+      <c r="A235" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A236" s="2" t="s">
+      <c r="A236" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A237" s="2" t="s">
+      <c r="A237" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A238" s="2" t="s">
+      <c r="A238" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A239" s="2" t="s">
+      <c r="A239" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A240" s="2" t="s">
+      <c r="A240" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A241" s="2" t="s">
+      <c r="A241" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A242" s="2" t="s">
+      <c r="A242" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2557,7 +2597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DBB0B2-47FD-44EC-91A3-3B6B77EE1CF7}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2626,7 +2668,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A15"/>
+      <selection activeCell="A15" sqref="A12:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5710,4 +5752,164 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2140A6-77AA-467D-BE7E-B73AD12B48D0}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5EC1A4-D2A0-4E03-AF49-353DDF02D94A}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>277</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>